<commit_message>
Updated my_app layout and sudokustats.db
</commit_message>
<xml_diff>
--- a/Sudoku Puzzle.xlsx
+++ b/Sudoku Puzzle.xlsx
@@ -457,91 +457,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" customHeight="1">
-      <c r="A1" s="1">
-        <v>6</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="2">
-        <v>3</v>
-      </c>
+      <c r="C1" s="2"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="18" customHeight="1">
+      <c r="A2" s="4">
         <v>8</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2">
-        <v>7</v>
-      </c>
-      <c r="I1" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="18" customHeight="1">
-      <c r="A2" s="4"/>
       <c r="B2" s="5"/>
-      <c r="C2" s="5">
-        <v>7</v>
-      </c>
+      <c r="C2" s="5"/>
       <c r="D2" s="4">
-        <v>5</v>
-      </c>
-      <c r="E2" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3</v>
+      </c>
       <c r="F2" s="5"/>
-      <c r="G2" s="4">
-        <v>3</v>
-      </c>
+      <c r="G2" s="4"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
+      <c r="I2" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1">
       <c r="A3" s="4"/>
       <c r="B3" s="5">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5">
+        <v>8</v>
+      </c>
+      <c r="G3" s="4">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5">
+        <v>9</v>
+      </c>
+      <c r="I3" s="6">
         <v>1</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4">
+    </row>
+    <row r="4" spans="1:9" ht="18" customHeight="1">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
-        <v>4</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="4">
-        <v>5</v>
-      </c>
-      <c r="H3" s="5">
-        <v>6</v>
-      </c>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="2">
-        <v>6</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="1">
+      <c r="H4" s="2"/>
+      <c r="I4" s="3">
         <v>9</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1">
       <c r="A5" s="4"/>
       <c r="B5" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="4">
@@ -550,86 +540,84 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="5">
-        <v>4</v>
-      </c>
+      <c r="H5" s="5"/>
       <c r="I5" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="5">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="5">
-        <v>3</v>
-      </c>
-      <c r="F6" s="5">
         <v>9</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1">
       <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
-        <v>9</v>
-      </c>
       <c r="C7" s="2">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2">
-        <v>3</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1"/>
       <c r="H7" s="2"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1">
       <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5">
+        <v>6</v>
+      </c>
       <c r="C8" s="5"/>
       <c r="D8" s="4">
         <v>9</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5">
+        <v>4</v>
+      </c>
       <c r="G8" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="6"/>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8">
-        <v>2</v>
-      </c>
-      <c r="C9" s="8">
-        <v>8</v>
-      </c>
+      <c r="A9" s="7">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="7">
-        <v>7</v>
-      </c>
+      <c r="G9" s="7"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
+      <c r="I9" s="9">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated html layout of my_app
</commit_message>
<xml_diff>
--- a/Sudoku Puzzle.xlsx
+++ b/Sudoku Puzzle.xlsx
@@ -457,166 +457,244 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" customHeight="1">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
+      <c r="C1" s="2">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="1">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="18" customHeight="1">
       <c r="A2" s="4">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5">
+        <v>3</v>
+      </c>
+      <c r="G2" s="4">
+        <v>9</v>
+      </c>
+      <c r="H2" s="5">
+        <v>4</v>
+      </c>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="18" customHeight="1">
+      <c r="A3" s="4">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
         <v>8</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="4">
+      <c r="D3" s="4">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5">
+        <v>7</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="4">
+        <v>2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6">
         <v>6</v>
       </c>
-      <c r="E2" s="5">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6">
+    </row>
+    <row r="4" spans="1:9" ht="18" customHeight="1">
+      <c r="A4" s="1">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="18" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5">
-        <v>8</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="E4" s="2">
         <v>6</v>
       </c>
-      <c r="H3" s="5">
-        <v>9</v>
-      </c>
-      <c r="I3" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2"/>
       <c r="F4" s="2">
         <v>5</v>
       </c>
       <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2</v>
+      </c>
+      <c r="I4" s="3">
         <v>3</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3">
-        <v>9</v>
-      </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1">
-      <c r="A5" s="4"/>
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
       <c r="B5" s="5">
+        <v>6</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>7</v>
+      </c>
+      <c r="G5" s="4">
         <v>8</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6">
+      <c r="H5" s="5">
         <v>5</v>
       </c>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1">
-      <c r="A6" s="4"/>
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
       <c r="B6" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="5">
         <v>9</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5">
+        <v>8</v>
+      </c>
       <c r="G6" s="4">
-        <v>1</v>
-      </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="H6" s="5">
+        <v>7</v>
+      </c>
+      <c r="I6" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1">
       <c r="A7" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1">
+        <v>7</v>
+      </c>
       <c r="E7" s="2">
         <v>5</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
+      <c r="H7" s="2">
+        <v>9</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1">
-      <c r="A8" s="4"/>
+      <c r="A8" s="4">
+        <v>9</v>
+      </c>
       <c r="B8" s="5">
-        <v>6</v>
-      </c>
-      <c r="C8" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="5">
+        <v>3</v>
+      </c>
       <c r="D8" s="4">
-        <v>9</v>
-      </c>
-      <c r="E8" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2</v>
+      </c>
       <c r="F8" s="5">
         <v>4</v>
       </c>
       <c r="G8" s="4">
         <v>5</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
+      <c r="H8" s="5">
+        <v>6</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1">
       <c r="A9" s="7">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8">
         <v>5</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="8">
+        <v>6</v>
+      </c>
+      <c r="D9" s="7">
+        <v>9</v>
+      </c>
       <c r="E9" s="8">
-        <v>1</v>
-      </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7">
+        <v>4</v>
+      </c>
+      <c r="H9" s="8">
+        <v>8</v>
+      </c>
       <c r="I9" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>